<commit_message>
vault backup: 2024-12-29 22:26:05
</commit_message>
<xml_diff>
--- a/Business Development/Startup Budget/attachments/Startup_Budget_Template.xlsx
+++ b/Business Development/Startup Budget/attachments/Startup_Budget_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffviolo/Library/Mobile Documents/iCloud~md~obsidian/Documents/Luminous/Business Development/Startup Budget/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBBEB2A-F4EB-2C42-ABF9-C9E7311A6846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6829D892-EEC4-E04A-84D4-AB9649A9F8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15000" yWindow="13880" windowWidth="28960" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="2960" windowWidth="28960" windowHeight="15420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Startup Budget" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Category</t>
   </si>
@@ -139,7 +139,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -448,7 +448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -586,113 +586,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
       <c r="D1" s="5"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>5000</v>
-      </c>
-      <c r="C2" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1">
-        <v>5000</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3000</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>5000</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>10000</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-    </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="4">
-        <f>SUM(B2:B8)</f>
-        <v>28000</v>
-      </c>
-      <c r="C9" s="4">
-        <f>SUM(C2:C8)</f>
-        <v>18200</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A11" s="3"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="4">
-        <f>(C9*12)+B9</f>
-        <v>246400</v>
-      </c>
+      <c r="C11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>